<commit_message>
Merged PR 3806: Merge fix/fix-integration-tests to develop
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Syndication_ValidFile5.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ProprietaryDataFiles/Syndication_ValidFile5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\bbotelho\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\ProprietaryDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{065B4524-1C0D-41DE-8755-2310DBF951FA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7120D149-04F3-4492-B29E-C811F734D847}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,6 +657,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -666,20 +672,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1058,9 +1058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="15" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="24" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1114,24 +1114,24 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43" t="str">
+      <c r="D2" s="37"/>
+      <c r="E2" s="41" t="str">
         <f>IF(COUNTA($E$3:$E10) &gt; 0, "Errors", "")</f>
         <v/>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="4"/>
@@ -1149,7 +1149,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1160,12 +1160,12 @@
         <v>4</v>
       </c>
       <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="40"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="4"/>
@@ -1183,7 +1183,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -1194,12 +1194,12 @@
         <v>6</v>
       </c>
       <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="4"/>
@@ -1217,7 +1217,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
@@ -1228,12 +1228,12 @@
         <v>6</v>
       </c>
       <c r="D5" s="35"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="4"/>
@@ -1251,7 +1251,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
@@ -1262,12 +1262,12 @@
         <v>9</v>
       </c>
       <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="4"/>
@@ -1285,23 +1285,23 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="12">
-        <v>24.1234</v>
+        <v>10</v>
       </c>
       <c r="C7" s="34">
         <v>25.123000000000001</v>
       </c>
       <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="40"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="4"/>
@@ -1319,7 +1319,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -1330,12 +1330,12 @@
         <v>12</v>
       </c>
       <c r="D8" s="35"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="4"/>
@@ -1353,7 +1353,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1364,12 +1364,12 @@
         <v>12</v>
       </c>
       <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="4"/>
@@ -1387,23 +1387,23 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="38"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="4"/>
@@ -1421,7 +1421,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26" ht="24" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="3"/>
       <c r="C11" s="17"/>
@@ -1449,7 +1449,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -33161,14 +33161,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="18">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E2:J2"/>
-    <mergeCell ref="E3:J3"/>
-    <mergeCell ref="E5:J5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:J6"/>
     <mergeCell ref="E10:J10"/>
@@ -33179,6 +33171,14 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E7:J7"/>
     <mergeCell ref="E8:J8"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="E3:J3"/>
+    <mergeCell ref="E5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B10 E3:E10">
     <cfRule type="expression" dxfId="6" priority="36">

</xml_diff>